<commit_message>
Updated sprint backlog day 3
</commit_message>
<xml_diff>
--- a/Sprint1/Sprint 1 Backlog.xlsx
+++ b/Sprint1/Sprint 1 Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>SPRINT 1 BACKLOG</t>
   </si>
@@ -49,22 +49,34 @@
     <t>Backend Requirements Gathering</t>
   </si>
   <si>
+    <t>Backend Team</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
     <t>Frontend Requirements Gathering</t>
   </si>
   <si>
+    <t>Frontend Team</t>
+  </si>
+  <si>
     <t>Completed</t>
   </si>
   <si>
     <t>Create sequence diagram for game</t>
   </si>
   <si>
+    <t>Melvin</t>
+  </si>
+  <si>
     <t>Create wireframe designs for the site</t>
   </si>
   <si>
     <t>Create user stories</t>
   </si>
   <si>
-    <t>In progress</t>
+    <t>Ruth, Kayla</t>
   </si>
   <si>
     <t>Create preliminary UI design</t>
@@ -76,12 +88,21 @@
     <t>Finalise branding</t>
   </si>
   <si>
+    <t>Alex</t>
+  </si>
+  <si>
     <t>Create branding pack</t>
   </si>
   <si>
     <t>Analyse design justifications</t>
   </si>
   <si>
+    <t>Ruth</t>
+  </si>
+  <si>
+    <t>Not started</t>
+  </si>
+  <si>
     <t>Fully understand ethics proposal and its implications and share with the team</t>
   </si>
   <si>
@@ -100,15 +121,21 @@
     <t>Front-end interface implementation: Start page</t>
   </si>
   <si>
+    <t>Kayla</t>
+  </si>
+  <si>
+    <t>In progess</t>
+  </si>
+  <si>
+    <t>Front-end interface implementation: Single player main quiz page</t>
+  </si>
+  <si>
+    <t>Front-end interface implementation:  Quiz ended page</t>
+  </si>
+  <si>
     <t>Not Started</t>
   </si>
   <si>
-    <t>Front-end interface implementation: Single player main quiz page</t>
-  </si>
-  <si>
-    <t>Front-end interface implementation:  Quiz ended page</t>
-  </si>
-  <si>
     <t>Research implementation methods of continuous Integration and continuous delivery</t>
   </si>
   <si>
@@ -122,6 +149,30 @@
   </si>
   <si>
     <t>Load data into mongoDB</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Create timer and countdown component</t>
+  </si>
+  <si>
+    <t>Danyal</t>
+  </si>
+  <si>
+    <t>Create leaderboard component</t>
+  </si>
+  <si>
+    <t>Create answer buttons and question bar component</t>
+  </si>
+  <si>
+    <t>Create header and main menu components</t>
+  </si>
+  <si>
+    <t>Create player identifier component</t>
+  </si>
+  <si>
+    <t>Nazat</t>
   </si>
 </sst>
 </file>
@@ -153,7 +204,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +215,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3C78D8"/>
+        <bgColor rgb="FF3C78D8"/>
       </patternFill>
     </fill>
   </fills>
@@ -187,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -206,10 +275,16 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -482,284 +557,410 @@
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5">
+        <v>8.0</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5">
+        <v>8.0</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5">
+        <v>6.0</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5">
+        <v>7.0</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5">
+        <v>8.0</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="5">
+        <v>8.0</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8.0</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5">
+        <v>5.0</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="5">
+        <v>5.0</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="5">
+        <v>7.0</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>23</v>
+      <c r="A13" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="5">
+        <v>5.0</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="s">
-        <v>25</v>
+      <c r="A14" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="5">
+        <v>9.0</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="5">
+        <v>4.0</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="2"/>
+      <c r="A16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="5">
+        <v>7.0</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="2"/>
+      <c r="A17" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="5">
+        <v>9.0</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="2"/>
+      <c r="A18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="5">
+        <v>5.0</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>32</v>
+      <c r="A19" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="5">
+        <v>8.0</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="5">
+        <v>7.0</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="5">
+        <v>8.0</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="8"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="A22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="5">
+        <v>8.0</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="8"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="A23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="5">
+        <v>8.0</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="8"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="5">
+        <v>8.0</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
     <row r="25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="A25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="5">
+        <v>7.0</v>
+      </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
     <row r="26">
-      <c r="A26" s="8"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="A26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="5">
+        <v>6.0</v>
+      </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
     <row r="27">
-      <c r="A27" s="8"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -768,7 +969,7 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="8"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -777,7 +978,7 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="8"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -786,7 +987,7 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30">
-      <c r="A30" s="8"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -795,7 +996,7 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31">
-      <c r="A31" s="8"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -804,7 +1005,7 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32">
-      <c r="A32" s="8"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -813,7 +1014,7 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="8"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -822,7 +1023,7 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34">
-      <c r="A34" s="8"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -831,7 +1032,7 @@
       <c r="G34" s="2"/>
     </row>
     <row r="35">
-      <c r="A35" s="8"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -840,7 +1041,7 @@
       <c r="G35" s="2"/>
     </row>
     <row r="36">
-      <c r="A36" s="8"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -849,7 +1050,7 @@
       <c r="G36" s="2"/>
     </row>
     <row r="37">
-      <c r="A37" s="8"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -858,7 +1059,7 @@
       <c r="G37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="8"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -867,7 +1068,7 @@
       <c r="G38" s="2"/>
     </row>
     <row r="39">
-      <c r="A39" s="8"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -876,7 +1077,7 @@
       <c r="G39" s="2"/>
     </row>
     <row r="40">
-      <c r="A40" s="8"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -885,7 +1086,7 @@
       <c r="G40" s="2"/>
     </row>
     <row r="41">
-      <c r="A41" s="8"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>

</xml_diff>